<commit_message>
add code to prod
</commit_message>
<xml_diff>
--- a/Projects/NESTLEIL/Tests/Data/test_case_1.xlsx
+++ b/Projects/NESTLEIL/Tests/Data/test_case_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,26 +13,29 @@
     <sheet name="scif" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">all_products!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$54</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$K$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$J$54</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$K$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">scif!$A$1:$K$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">scif!$A$1:$K$5</definedName>
@@ -44,6 +47,8 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$K$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$K$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$K$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$K$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">scif!$A$1:$K$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -55,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t xml:space="preserve">probe_match_fk</t>
   </si>
@@ -105,6 +110,12 @@
     <t xml:space="preserve">manufacturer_name</t>
   </si>
   <si>
+    <t xml:space="preserve">trax_category_fk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_fk</t>
+  </si>
+  <si>
     <t xml:space="preserve">Product 1</t>
   </si>
   <si>
@@ -139,6 +150,21 @@
   </si>
   <si>
     <t xml:space="preserve">Product 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product 13</t>
   </si>
   <si>
     <t xml:space="preserve">facings</t>
@@ -190,7 +216,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +231,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -244,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -261,11 +299,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,7 +327,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -349,31 +395,36 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.1530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,8 +657,536 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>101</v>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I8" s="4" t="n">
+        <f aca="false">VLOOKUP(H8, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>102</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <f aca="false">VLOOKUP(H9, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>103</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I10" s="4" t="n">
+        <f aca="false">VLOOKUP(H10, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>104</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <f aca="false">VLOOKUP(H11, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>105</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <f aca="false">VLOOKUP(H12, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>106</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I13" s="4" t="n">
+        <f aca="false">VLOOKUP(H13, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>107</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4" t="n">
+        <f aca="false">VLOOKUP(H14, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>108</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <f aca="false">VLOOKUP(H15, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
+        <v>109</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4" t="n">
+        <f aca="false">VLOOKUP(H16, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>110</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <f aca="false">VLOOKUP(H17, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="n">
+        <v>111</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I18" s="4" t="n">
+        <f aca="false">VLOOKUP(H18, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
+        <v>112</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <f aca="false">VLOOKUP(H19, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
+        <v>113</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I20" s="4" t="n">
+        <f aca="false">VLOOKUP(H20, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>114</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <f aca="false">VLOOKUP(H21, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="n">
+        <v>115</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I22" s="4" t="n">
+        <f aca="false">VLOOKUP(H22, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>5</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <f aca="false">VLOOKUP(H23, all_products!$A$2:$C$20, 2, 0)</f>
+        <v>13</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J52"/>
+  <autoFilter ref="A1:J54"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -624,44 +1203,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,19 +1259,25 @@
         <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -695,19 +1288,25 @@
         <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,19 +1317,25 @@
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>18</v>
+      <c r="H4" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -741,19 +1346,25 @@
         <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -764,19 +1375,25 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>3</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,19 +1404,25 @@
         <v>3</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>25</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,19 +1433,25 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>25</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,22 +1462,175 @@
         <v>13</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="4" t="n">
         <v>25</v>
       </c>
+      <c r="I10" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I12" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I13" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I14" s="4" t="n">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I14"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -856,6 +1638,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -864,23 +1647,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K37" activeCellId="0" sqref="K37"/>
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,16 +1676,16 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>11</v>
@@ -917,49 +1702,56 @@
       <c r="K1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="n">
+      <c r="L1" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="n">
         <v>153</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A2,matches!$H$2:$H$101,$B2)</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A2,matches!$H$2:$H$101,$B2, matches!$F$2:$F$101, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A2,matches!$H$2:$H$101,$B2)</f>
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A2,matches!$H$2:$H$101,$B2, matches!$F$2:$F$101, 1)</f>
-        <v>5</v>
-      </c>
-      <c r="G2" s="5" t="str">
-        <f aca="false">VLOOKUP(B2,all_products!$A$2:$C$10, 3, 0)</f>
+      <c r="C2" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A2,matches!$H$2:$H$103,$B2)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A2,matches!$H$2:$H$103,$B2, matches!$F$2:$F$103, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A2,matches!$H$2:$H$103,$B2)</f>
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A2,matches!$H$2:$H$103,$B2, matches!$F$2:$F$103, 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="str">
+        <f aca="false">VLOOKUP(B2,all_products!$A$2:$C$20, 3, 0)</f>
         <v>Product 2</v>
       </c>
-      <c r="H2" s="5" t="str">
-        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$10, 4, 0)</f>
+      <c r="H2" s="6" t="str">
+        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$20, 4, 0)</f>
         <v>Snacks</v>
       </c>
-      <c r="I2" s="5" t="n">
-        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$10, 5, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$10, 6, 0)</f>
-        <v>3</v>
-      </c>
-      <c r="K2" s="5" t="str">
-        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$10, 7, 0)</f>
+      <c r="I2" s="6" t="n">
+        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J2" s="6" t="n">
+        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K2" s="6" t="str">
+        <f aca="false">VLOOKUP($B2, all_products!$A$2:$G$20, 7, 0)</f>
         <v>Osem</v>
+      </c>
+      <c r="L2" s="6" t="n">
+        <f aca="false">VLOOKUP($B2, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>8</v>
       </c>
       <c r="AMC2" s="0"/>
       <c r="AMD2" s="0"/>
@@ -970,48 +1762,52 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="n">
+    <row r="3" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>157</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A3,matches!$H$2:$H$101,$B3)</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A3,matches!$H$2:$H$101,$B3, matches!$F$2:$F$101, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A3,matches!$H$2:$H$101,$B3)</f>
+      <c r="C3" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A3,matches!$H$2:$H$103,$B3)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A3,matches!$H$2:$H$103,$B3, matches!$F$2:$F$103, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A3,matches!$H$2:$H$103,$B3)</f>
         <v>15</v>
       </c>
-      <c r="F3" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A3,matches!$H$2:$H$101,$B3, matches!$F$2:$F$101, 1)</f>
+      <c r="F3" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A3,matches!$H$2:$H$103,$B3, matches!$F$2:$F$103, 1)</f>
         <v>15</v>
       </c>
-      <c r="G3" s="5" t="str">
-        <f aca="false">VLOOKUP(B3,all_products!$A$2:$C$10, 3, 0)</f>
+      <c r="G3" s="6" t="str">
+        <f aca="false">VLOOKUP(B3,all_products!$A$2:$C$20, 3, 0)</f>
         <v>Product 3</v>
       </c>
-      <c r="H3" s="5" t="str">
-        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$10, 4, 0)</f>
+      <c r="H3" s="6" t="str">
+        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$20, 4, 0)</f>
         <v>Snacks</v>
       </c>
-      <c r="I3" s="5" t="n">
-        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$10, 5, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$10, 6, 0)</f>
-        <v>3</v>
-      </c>
-      <c r="K3" s="5" t="str">
-        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$10, 7, 0)</f>
+      <c r="I3" s="6" t="n">
+        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J3" s="6" t="n">
+        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K3" s="6" t="str">
+        <f aca="false">VLOOKUP($B3, all_products!$A$2:$G$20, 7, 0)</f>
         <v>Osem</v>
+      </c>
+      <c r="L3" s="6" t="n">
+        <f aca="false">VLOOKUP($B3, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>7</v>
       </c>
       <c r="AMC3" s="0"/>
       <c r="AMD3" s="0"/>
@@ -1022,48 +1818,52 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="n">
+    <row r="4" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>253</v>
       </c>
-      <c r="C4" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A4,matches!$H$2:$H$101,$B4)</f>
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A4,matches!$H$2:$H$101,$B4, matches!$F$2:$F$101, 1)</f>
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A4,matches!$H$2:$H$101,$B4)</f>
+      <c r="C4" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A4,matches!$H$2:$H$103,$B4)</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A4,matches!$H$2:$H$103,$B4, matches!$F$2:$F$103, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A4,matches!$H$2:$H$103,$B4)</f>
         <v>40</v>
       </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A4,matches!$H$2:$H$101,$B4, matches!$F$2:$F$101, 1)</f>
+      <c r="F4" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A4,matches!$H$2:$H$103,$B4, matches!$F$2:$F$103, 1)</f>
         <v>40</v>
       </c>
-      <c r="G4" s="5" t="str">
-        <f aca="false">VLOOKUP(B4,all_products!$A$2:$C$10, 3, 0)</f>
+      <c r="G4" s="6" t="str">
+        <f aca="false">VLOOKUP(B4,all_products!$A$2:$C$20, 3, 0)</f>
         <v>Product 4</v>
       </c>
-      <c r="H4" s="5" t="str">
-        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$10, 4, 0)</f>
+      <c r="H4" s="6" t="str">
+        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$20, 4, 0)</f>
         <v>Sabra</v>
       </c>
-      <c r="I4" s="5" t="n">
-        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$10, 5, 0)</f>
-        <v>2</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$10, 6, 0)</f>
-        <v>3</v>
-      </c>
-      <c r="K4" s="5" t="str">
-        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$10, 7, 0)</f>
+      <c r="I4" s="6" t="n">
+        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>7</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K4" s="6" t="str">
+        <f aca="false">VLOOKUP($B4, all_products!$A$2:$G$20, 7, 0)</f>
         <v>Osem</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <f aca="false">VLOOKUP($B4, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>7</v>
       </c>
       <c r="AMC4" s="0"/>
       <c r="AMD4" s="0"/>
@@ -1074,48 +1874,52 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A5,matches!$H$2:$H$101,$B5)</f>
-        <v>2</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$J$2:$J$101,matches!$B$2:$B$101,$A5,matches!$H$2:$H$101,$B5, matches!$F$2:$F$101, 1)</f>
+    <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A5,matches!$H$2:$H$103,$B5)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A5,matches!$H$2:$H$103,$B5, matches!$F$2:$F$103, 1)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A5,matches!$H$2:$H$101,$B5)</f>
+      <c r="E5" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A5,matches!$H$2:$H$103,$B5)</f>
         <v>6</v>
       </c>
-      <c r="F5" s="5" t="n">
-        <f aca="false">SUMIFS(matches!$I$2:$I$101,matches!$B$2:$B$101,$A5,matches!$H$2:$H$101,$B5, matches!$F$2:$F$101, 1)</f>
+      <c r="F5" s="6" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A5,matches!$H$2:$H$103,$B5, matches!$F$2:$F$103, 1)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="5" t="str">
-        <f aca="false">VLOOKUP(B5,all_products!$A$2:$C$10, 3, 0)</f>
+      <c r="G5" s="6" t="str">
+        <f aca="false">VLOOKUP(B5,all_products!$A$2:$C$20, 3, 0)</f>
         <v>Product 6</v>
       </c>
-      <c r="H5" s="5" t="str">
-        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$10, 4, 0)</f>
+      <c r="H5" s="6" t="str">
+        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$20, 4, 0)</f>
         <v>Snacks</v>
       </c>
-      <c r="I5" s="5" t="n">
-        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$10, 5, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$10, 6, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="5" t="str">
-        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$10, 7, 0)</f>
+      <c r="I5" s="6" t="n">
+        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="6" t="str">
+        <f aca="false">VLOOKUP($B5, all_products!$A$2:$G$20, 7, 0)</f>
         <v>Non-Osem</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <f aca="false">VLOOKUP($B5, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>100</v>
       </c>
       <c r="AMC5" s="0"/>
       <c r="AMD5" s="0"/>
@@ -1125,6 +1929,294 @@
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A6,matches!$H$2:$H$103,$B6)</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A6,matches!$H$2:$H$103,$B6, matches!$F$2:$F$103, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A6,matches!$H$2:$H$103,$B6)</f>
+        <v>15</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A6,matches!$H$2:$H$103,$B6, matches!$F$2:$F$103, 1)</f>
+        <v>15</v>
+      </c>
+      <c r="G6" s="7" t="str">
+        <f aca="false">VLOOKUP(B6,all_products!$A$2:$C$20, 3, 0)</f>
+        <v>Product 9</v>
+      </c>
+      <c r="H6" s="7" t="str">
+        <f aca="false">VLOOKUP($B6, all_products!$A$2:$G$20, 4, 0)</f>
+        <v>Snacks</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <f aca="false">VLOOKUP($B6, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <f aca="false">VLOOKUP($B6, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K6" s="7" t="str">
+        <f aca="false">VLOOKUP($B6, all_products!$A$2:$G$20, 7, 0)</f>
+        <v>Osem</v>
+      </c>
+      <c r="L6" s="7" t="n">
+        <f aca="false">VLOOKUP($B6, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A7,matches!$H$2:$H$103,$B7)</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A7,matches!$H$2:$H$103,$B7, matches!$F$2:$F$103, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A7,matches!$H$2:$H$103,$B7)</f>
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A7,matches!$H$2:$H$103,$B7, matches!$F$2:$F$103, 1)</f>
+        <v>15</v>
+      </c>
+      <c r="G7" s="7" t="str">
+        <f aca="false">VLOOKUP(B7,all_products!$A$2:$C$20, 3, 0)</f>
+        <v>Product 10</v>
+      </c>
+      <c r="H7" s="7" t="str">
+        <f aca="false">VLOOKUP($B7, all_products!$A$2:$G$20, 4, 0)</f>
+        <v>Snacks</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <f aca="false">VLOOKUP($B7, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <f aca="false">VLOOKUP($B7, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="7" t="str">
+        <f aca="false">VLOOKUP($B7, all_products!$A$2:$G$20, 7, 0)</f>
+        <v>Osem</v>
+      </c>
+      <c r="L7" s="7" t="n">
+        <f aca="false">VLOOKUP($B7, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A8,matches!$H$2:$H$103,$B8)</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A8,matches!$H$2:$H$103,$B8, matches!$F$2:$F$103, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A8,matches!$H$2:$H$103,$B8)</f>
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A8,matches!$H$2:$H$103,$B8, matches!$F$2:$F$103, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="str">
+        <f aca="false">VLOOKUP(B8,all_products!$A$2:$C$20, 3, 0)</f>
+        <v>Product 11</v>
+      </c>
+      <c r="H8" s="7" t="str">
+        <f aca="false">VLOOKUP($B8, all_products!$A$2:$G$20, 4, 0)</f>
+        <v>Snacks</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <f aca="false">VLOOKUP($B8, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <f aca="false">VLOOKUP($B8, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K8" s="7" t="str">
+        <f aca="false">VLOOKUP($B8, all_products!$A$2:$G$20, 7, 0)</f>
+        <v>Osem</v>
+      </c>
+      <c r="L8" s="7" t="n">
+        <f aca="false">VLOOKUP($B8, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A9,matches!$H$2:$H$103,$B9)</f>
+        <v>3</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A9,matches!$H$2:$H$103,$B9, matches!$F$2:$F$103, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A9,matches!$H$2:$H$103,$B9)</f>
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A9,matches!$H$2:$H$103,$B9, matches!$F$2:$F$103, 1)</f>
+        <v>15</v>
+      </c>
+      <c r="G9" s="7" t="str">
+        <f aca="false">VLOOKUP(B9,all_products!$A$2:$C$20, 3, 0)</f>
+        <v>Product 12</v>
+      </c>
+      <c r="H9" s="7" t="str">
+        <f aca="false">VLOOKUP($B9, all_products!$A$2:$G$20, 4, 0)</f>
+        <v>Snacks</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <f aca="false">VLOOKUP($B9, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <f aca="false">VLOOKUP($B9, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K9" s="7" t="str">
+        <f aca="false">VLOOKUP($B9, all_products!$A$2:$G$20, 7, 0)</f>
+        <v>Osem</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <f aca="false">VLOOKUP($B9, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A10,matches!$H$2:$H$103,$B10)</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A10,matches!$H$2:$H$103,$B10, matches!$F$2:$F$103, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A10,matches!$H$2:$H$103,$B10)</f>
+        <v>15</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A10,matches!$H$2:$H$103,$B10, matches!$F$2:$F$103, 1)</f>
+        <v>15</v>
+      </c>
+      <c r="G10" s="7" t="str">
+        <f aca="false">VLOOKUP(B10,all_products!$A$2:$C$20, 3, 0)</f>
+        <v>Product 13</v>
+      </c>
+      <c r="H10" s="7" t="str">
+        <f aca="false">VLOOKUP($B10, all_products!$A$2:$G$20, 4, 0)</f>
+        <v>Snacks</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <f aca="false">VLOOKUP($B10, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <f aca="false">VLOOKUP($B10, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="K10" s="7" t="str">
+        <f aca="false">VLOOKUP($B10, all_products!$A$2:$G$20, 7, 0)</f>
+        <v>Osem</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <f aca="false">VLOOKUP($B10, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A11,matches!$H$2:$H$103,$B11)</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$J$2:$J$103,matches!$B$2:$B$103,$A11,matches!$H$2:$H$103,$B11, matches!$F$2:$F$103, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A11,matches!$H$2:$H$103,$B11)</f>
+        <v>13</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <f aca="false">SUMIFS(matches!$I$2:$I$103,matches!$B$2:$B$103,$A11,matches!$H$2:$H$103,$B11, matches!$F$2:$F$103, 1)</f>
+        <v>13</v>
+      </c>
+      <c r="G11" s="7" t="str">
+        <f aca="false">VLOOKUP(B11,all_products!$A$2:$C$20, 3, 0)</f>
+        <v>Product 8</v>
+      </c>
+      <c r="H11" s="7" t="str">
+        <f aca="false">VLOOKUP($B11, all_products!$A$2:$G$20, 4, 0)</f>
+        <v>Sabra</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <f aca="false">VLOOKUP($B11, all_products!$A$2:$G$20, 5, 0)</f>
+        <v>8</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <f aca="false">VLOOKUP($B11, all_products!$A$2:$G$20, 6, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="7" t="str">
+        <f aca="false">VLOOKUP($B11, all_products!$A$2:$G$20, 7, 0)</f>
+        <v>Non-Osem</v>
+      </c>
+      <c r="L11" s="7" t="n">
+        <f aca="false">VLOOKUP($B11, all_products!$A$2:$I$20, 9, 0)</f>
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K5"/>

</xml_diff>